<commit_message>
Add Excel Data Cleaning Assignment File
</commit_message>
<xml_diff>
--- a/DataCleaningAssignment.xlsx
+++ b/DataCleaningAssignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahta\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796FC25D-C478-40B1-A301-256F7DFF2199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A8E5E1-4603-4AB7-B352-EF213525D75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{786AFE3D-C85D-49F9-9476-D1ECC1602DC4}"/>
   </bookViews>
@@ -549,51 +549,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1) TRIM : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TRIM function usually used when we've to remove extra spaces. It removes extra spaces</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4) MID : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MID function extracts characters from any position in a text. Syntax of this function</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5) CONCAT : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CONCAT function joins multiple texts into one. Syntax of this function</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">is </t>
     </r>
     <r>
@@ -2418,17 +2373,94 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">2) LEFT : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LEFT function extracts a specific number or characters from the beginning of the text.</t>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1) TRIM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : TRIM function usually used when we've to remove extra spaces. It removes extra spaces</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2) LEFT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : LEFT function extracts a specific number or characters from the beginning of the text.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4) MID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : MID function extracts characters from any position in a text. Syntax of this function</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5) CONCAT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : CONCAT function joins multiple texts into one. Syntax of this function</t>
     </r>
   </si>
 </sst>
@@ -2462,7 +2494,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="4" tint="0.79998168889431442"/>
+      <color theme="3" tint="0.89999084444715716"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2483,7 +2515,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2589,40 +2621,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2983,123 +3012,123 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3136,137 +3165,142 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D3"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="3">
         <v>4000</v>
       </c>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E5" s="11" t="s">
+      <c r="D5"/>
+      <c r="E5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="3">
         <v>5000</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E6" s="9" t="s">
+      <c r="D6"/>
+      <c r="E6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="3">
         <v>2500</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D7"/>
       <c r="E7" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E8" s="9" t="s">
+      <c r="D8"/>
+      <c r="E8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E9" s="2" t="s">
+      <c r="D9"/>
+      <c r="E9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="3">
         <v>5000</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="3">
         <v>4000</v>
       </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="3">
         <v>2500</v>
       </c>
     </row>
@@ -3304,100 +3338,112 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D5"/>
+      <c r="E5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D6"/>
+      <c r="E6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D7"/>
+      <c r="E7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D8"/>
+      <c r="E8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D9"/>
+      <c r="E9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D10"/>
+      <c r="E10" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D11"/>
+      <c r="E11" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D12"/>
+      <c r="E12" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D13"/>
+      <c r="E13" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14"/>
+      <c r="E14" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D15"/>
+      <c r="E15" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16"/>
+      <c r="E16" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="16" t="s">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="8" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E16" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="10" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3424,85 +3470,85 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>60</v>
+      <c r="D3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>62</v>
+      <c r="E4" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D5"/>
-      <c r="E5" s="9" t="s">
-        <v>63</v>
+      <c r="E5" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D6"/>
-      <c r="E6" s="10" t="s">
-        <v>64</v>
+      <c r="E6" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D7"/>
-      <c r="E7" s="9" t="s">
-        <v>65</v>
+      <c r="E7" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D8"/>
-      <c r="E8" s="9" t="s">
-        <v>66</v>
+      <c r="E8" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D9"/>
-      <c r="E9" s="9" t="s">
-        <v>67</v>
+      <c r="E9" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D10"/>
-      <c r="E10" s="9" t="s">
-        <v>110</v>
+      <c r="E10" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D11"/>
-      <c r="E11" s="9" t="s">
-        <v>71</v>
+      <c r="E11" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D12"/>
-      <c r="E12" s="9" t="s">
-        <v>72</v>
+      <c r="E12" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D13"/>
-      <c r="E13" s="9" t="s">
-        <v>68</v>
+      <c r="E13" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D14"/>
-      <c r="E14" s="9" t="s">
-        <v>69</v>
+      <c r="E14" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D15"/>
-      <c r="E15" s="10" t="s">
-        <v>70</v>
+      <c r="E15" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3535,208 +3581,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C2" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18">
+        <v>81</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18">
+        <v>121</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2">
+      <c r="B4" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="C4" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18">
+        <v>239</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18">
+        <v>500</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18">
+        <v>423</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <v>121</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" s="5" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18">
+        <v>160</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18">
+        <v>348</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18">
+        <v>152</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>239</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="10" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>500</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>423</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>160</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" s="20" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18">
+        <v>369</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11"/>
+      <c r="H11" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12"/>
+      <c r="H12" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13"/>
+      <c r="H13" s="8" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>348</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>152</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
-        <v>369</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H11" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H12" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H13" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3769,143 +3820,143 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D4" s="24" t="s">
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E7" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D5" s="7" t="s">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E8" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="9" t="s">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D10" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="7" t="s">
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="7" t="s">
+      <c r="E14" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="24" t="s">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E16" s="22" t="s">
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="8" t="s">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="9" t="s">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="9" t="s">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="9" t="s">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="8" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E21" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E22" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="10" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3935,113 +3986,113 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>139</v>
+      <c r="E2" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E4" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>140</v>
+      <c r="E4" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>152</v>
+      <c r="F5" s="13" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="5:6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="7" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E7" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>141</v>
+      <c r="E7" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>142</v>
+      <c r="F8" s="18" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="5:6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="10" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E10" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>143</v>
+      <c r="E10" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>144</v>
+      <c r="F11" s="13" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="5:6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="13" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E13" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>145</v>
+      <c r="E13" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>146</v>
+      <c r="F14" s="13" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="5:6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="16" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>147</v>
+      <c r="E16" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>148</v>
+      <c r="F17" s="10" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E18"/>
-      <c r="F18" s="9" t="s">
-        <v>149</v>
+      <c r="F18" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E19"/>
-      <c r="F19" s="9" t="s">
-        <v>151</v>
+      <c r="F19" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E20"/>
-      <c r="F20" s="10" t="s">
-        <v>150</v>
+      <c r="F20" s="8" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -4072,124 +4123,124 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E4" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F6" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F7" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E4" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="7" t="s">
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F9" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F6" s="9" t="s">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F7" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E9" s="7" t="s">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F13" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="9" t="s">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F14" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="4"/>
+      <c r="E16" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F11" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E12" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E13" s="7" t="s">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="7"/>
+      <c r="E19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F14" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E15" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="17"/>
-      <c r="E16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="F19" s="18" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E18" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="23"/>
-      <c r="E19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>